<commit_message>
Agregue precios al Excel
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>PCS</t>
   </si>
@@ -53,6 +53,33 @@
   </si>
   <si>
     <t>1 mm de 100 metros</t>
+  </si>
+  <si>
+    <t>Cableados</t>
+  </si>
+  <si>
+    <t>Contenido de la Of</t>
+  </si>
+  <si>
+    <t>Terreno</t>
+  </si>
+  <si>
+    <t>Puerta Exterior</t>
+  </si>
+  <si>
+    <t>U$S 59.990</t>
+  </si>
+  <si>
+    <t>Total de la ventanas del Exter</t>
+  </si>
+  <si>
+    <t>U$S16,730</t>
+  </si>
+  <si>
+    <t>Ventana interior</t>
+  </si>
+  <si>
+    <t>U$S78</t>
   </si>
 </sst>
 </file>
@@ -139,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -154,6 +181,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,8 +504,10 @@
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -488,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -505,7 +538,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -520,7 +553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -535,15 +568,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Segui agregando precios y productos
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7800"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="10155" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>PCS</t>
   </si>
@@ -80,6 +80,48 @@
   </si>
   <si>
     <t>U$S78</t>
+  </si>
+  <si>
+    <t>Sofa</t>
+  </si>
+  <si>
+    <t>Butacas</t>
+  </si>
+  <si>
+    <t>TV LED 40"</t>
+  </si>
+  <si>
+    <t>U$S274</t>
+  </si>
+  <si>
+    <t>TV LED 32"</t>
+  </si>
+  <si>
+    <t>Sala Principal</t>
+  </si>
+  <si>
+    <t>U$S366</t>
+  </si>
+  <si>
+    <t>U$S134</t>
+  </si>
+  <si>
+    <t>u$s224</t>
+  </si>
+  <si>
+    <t>Cuarte de Baño</t>
+  </si>
+  <si>
+    <t>Puertas</t>
+  </si>
+  <si>
+    <t>U$S234</t>
+  </si>
+  <si>
+    <t>U$S280</t>
+  </si>
+  <si>
+    <t>Juego de loza inodora y pileta.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -183,8 +225,9 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +632,7 @@
       <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -604,6 +647,64 @@
       </c>
       <c r="E7" s="11" t="s">
         <v>21</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregue precios de la bandeja
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>PCS</t>
   </si>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t>Juego de loza inodora y pileta.</t>
+  </si>
+  <si>
+    <t>Conectores RJ45 CAT 5e</t>
+  </si>
+  <si>
+    <t>100 unidades 389 $</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.uy/MLU-450398185-switch-dell-security-sonicwall-nsa-5600-upg-plus-2-yr-fd-_JM</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>22.840$</t>
+  </si>
+  <si>
+    <t>Bandeja perforada Samet</t>
+  </si>
+  <si>
+    <t>3 metros x 257</t>
   </si>
 </sst>
 </file>
@@ -168,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -204,11 +225,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -223,11 +266,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,16 +593,19 @@
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -563,8 +614,17 @@
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="F1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -580,8 +640,17 @@
       <c r="E2" s="9">
         <v>499</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -595,8 +664,13 @@
       <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -610,102 +684,114 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregando url de los productos
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>PCS</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>3 metros x 257</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.uy/MLU-451914839-cable-de-red-utp-cat-5e-de-cobre-la-mejor-calidad-x-metro-_JM</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-609009072-conector-rj45-nexxt-cat5e-bolsa-c100pz-_JM</t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +179,22 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -248,10 +270,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -262,9 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -273,11 +293,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,10 +639,10 @@
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -634,37 +659,41 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>899</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>499</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="17" t="s">
         <v>38</v>
       </c>
@@ -700,34 +729,34 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -736,14 +765,14 @@
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -751,17 +780,17 @@
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -772,12 +801,13 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -786,7 +816,7 @@
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="1"/>
@@ -794,7 +824,14 @@
       <c r="F11" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregue precios de bandejas
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>PCS</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>3 metros x 257</t>
+  </si>
+  <si>
+    <t>Bandeja esq. perforada Samet</t>
+  </si>
+  <si>
+    <t>222 c/u</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.ar/MLA-608425204-curva-para-bandejas-portacables-ancho-30cm-m2-_JM</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.ar/MLA-668557795-bandeja-perforada-samet-50mm-x-3-mts-_JM</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +186,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -189,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -247,11 +267,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -276,8 +308,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,9 +636,10 @@
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -623,8 +664,11 @@
       <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -649,8 +693,11 @@
       <c r="H2" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I2" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -668,9 +715,14 @@
       <c r="G3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -687,13 +739,14 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -712,7 +765,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -729,7 +782,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -747,7 +800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -765,7 +818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -779,7 +832,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -794,7 +847,11 @@
       <c r="F11" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregue mas precios de los objetos de la oficina
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>PCS</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>3 metros x 257</t>
+  </si>
+  <si>
+    <t>Sala de reuniones</t>
+  </si>
+  <si>
+    <t>Cuarto de Servidores</t>
+  </si>
+  <si>
+    <t>Cuarto de Deposito</t>
+  </si>
+  <si>
+    <t>Cocina</t>
+  </si>
+  <si>
+    <t>Cuarto de Trabajo</t>
   </si>
 </sst>
 </file>
@@ -152,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +189,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -189,7 +212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -247,11 +270,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -273,11 +308,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,8 +830,36 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Termine de agregar los precios de todo lo que contine la oficina
</commit_message>
<xml_diff>
--- a/PRECIOS PROYECTO/Precios.xlsx
+++ b/PRECIOS PROYECTO/Precios.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>PCS</t>
   </si>
@@ -176,6 +177,18 @@
   </si>
   <si>
     <t>4 sillas de oficina</t>
+  </si>
+  <si>
+    <t>Deposito</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Maceta</t>
+  </si>
+  <si>
+    <t>Plantas</t>
   </si>
 </sst>
 </file>
@@ -641,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,13 +946,36 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A16" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="19">
+        <v>495</v>
+      </c>
+      <c r="C19" s="19">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -948,4 +984,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>